<commit_message>
Update: Se Actualiza Documentación
</commit_message>
<xml_diff>
--- a/6- VI_Trimestre/03- Plantilla_ISO_27002/01- Plantilla_ISO_27002.xlsx
+++ b/6- VI_Trimestre/03- Plantilla_ISO_27002/01- Plantilla_ISO_27002.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres_Olaya\Proyecto_Formativo\Kyukeisho_New\Kyukeisho_New\6- VI_Trimestre\03- Plantilla_ISO_27002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A834DDEE-8BEF-4DEC-9CD6-58F1DC9112E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC80E9DB-C6F9-42F8-8165-5CB64A1CFCFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D58A99C2-3583-4B04-BA4C-07AC581D820A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>Puntos Criticos</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>Por debajo del 30% calidad</t>
+  </si>
+  <si>
+    <t>Matriz De Calidad De Software</t>
+  </si>
+  <si>
+    <t>Matriz De Análisis De Riesgo</t>
   </si>
 </sst>
 </file>
@@ -308,7 +314,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +378,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -417,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="68">
     <border>
       <left/>
       <right/>
@@ -986,6 +998,248 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -995,13 +1249,10 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1041,12 +1292,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="7" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="7" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="7" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="7" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1154,27 +1401,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="32" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1184,16 +1431,58 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="32" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="55" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="55" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="55" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="62" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="62" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="63" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="67" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Énfasis3" xfId="3" builtinId="39"/>
@@ -1215,7 +1504,7 @@
         <scheme val="none"/>
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1239,7 +1528,7 @@
         <scheme val="none"/>
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1263,7 +1552,7 @@
         <scheme val="none"/>
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1287,7 +1576,7 @@
         <scheme val="none"/>
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1311,7 +1600,7 @@
         <scheme val="none"/>
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1335,7 +1624,7 @@
         <scheme val="none"/>
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1359,7 +1648,7 @@
         <scheme val="none"/>
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1383,7 +1672,7 @@
         <scheme val="none"/>
       </font>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -1791,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7014F898-5058-4D1B-9637-B21A5C3439BD}">
   <dimension ref="B1:J157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,1276 +2100,1320 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="74"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="79"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="77"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>1803170</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="82"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="77"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="82"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="77"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>43500</v>
       </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="82"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="11">
+      <c r="C9" s="82"/>
+      <c r="D9" s="10">
         <v>44000</v>
       </c>
-      <c r="E9" s="80"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="82"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="77"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="85"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="80"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="90"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="91" t="s">
+      <c r="D12" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="90"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="67" t="s">
+      <c r="C13" s="61"/>
+      <c r="D13" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="69"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="64"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="103"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="87"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="104"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="88"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="104"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="88"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="104"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="88"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="104"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="88"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="I24" s="18"/>
+      <c r="I24" s="17"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="104"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="18" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="88"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="17"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="105"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="18" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="89"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="I26" s="18"/>
+      <c r="I26" s="17"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E29" s="70" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
     </row>
     <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="102" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="24"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="25"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="24"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="94">
-        <v>1</v>
-      </c>
-      <c r="C32" s="92" t="s">
+      <c r="B32" s="103">
+        <v>1</v>
+      </c>
+      <c r="C32" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="57">
+      <c r="E32" s="52">
         <v>0.8</v>
       </c>
-      <c r="F32" s="60">
-        <v>1</v>
-      </c>
-      <c r="G32" s="27">
+      <c r="F32" s="55">
+        <v>1</v>
+      </c>
+      <c r="G32" s="26">
         <v>0.5</v>
       </c>
-      <c r="H32" s="28">
-        <v>1</v>
-      </c>
-      <c r="I32" s="29"/>
+      <c r="H32" s="27">
+        <v>1</v>
+      </c>
+      <c r="I32" s="104"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="94"/>
-      <c r="C33" s="92"/>
-      <c r="D33" s="30" t="s">
+      <c r="B33" s="103"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="27">
-        <v>1</v>
-      </c>
-      <c r="H33" s="28">
-        <v>1</v>
-      </c>
-      <c r="I33" s="31"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="26">
+        <v>1</v>
+      </c>
+      <c r="H33" s="27">
+        <v>1</v>
+      </c>
+      <c r="I33" s="105"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="94"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="30" t="s">
+      <c r="B34" s="103"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="57"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="27">
-        <v>1</v>
-      </c>
-      <c r="H34" s="28">
-        <v>1</v>
-      </c>
-      <c r="I34" s="31"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="26">
+        <v>1</v>
+      </c>
+      <c r="H34" s="27">
+        <v>1</v>
+      </c>
+      <c r="I34" s="105"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="94"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="30" t="s">
+      <c r="B35" s="103"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="57"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="27">
+      <c r="E35" s="52"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="26">
         <v>0.5</v>
       </c>
-      <c r="H35" s="28">
-        <v>1</v>
-      </c>
-      <c r="I35" s="32"/>
+      <c r="H35" s="27">
+        <v>1</v>
+      </c>
+      <c r="I35" s="106"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="95"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="30" t="s">
+      <c r="B36" s="107"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="57"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="33">
+      <c r="E36" s="52"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="29">
         <v>0.8</v>
       </c>
-      <c r="H36" s="28">
-        <v>1</v>
-      </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="35"/>
+      <c r="H36" s="27">
+        <v>1</v>
+      </c>
+      <c r="I36" s="108"/>
+      <c r="J36" s="30"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="98">
+      <c r="B37" s="109">
         <v>2</v>
       </c>
-      <c r="C37" s="96" t="s">
+      <c r="C37" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="58">
+      <c r="E37" s="53">
         <v>0.8</v>
       </c>
-      <c r="F37" s="63">
-        <v>1</v>
-      </c>
-      <c r="G37" s="33">
+      <c r="F37" s="58">
+        <v>1</v>
+      </c>
+      <c r="G37" s="29">
         <v>0.9</v>
       </c>
-      <c r="H37" s="28">
-        <v>1</v>
-      </c>
-      <c r="I37" s="31"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="27">
+        <v>1</v>
+      </c>
+      <c r="I37" s="105"/>
+      <c r="J37" s="30"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="94"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="30" t="s">
+      <c r="B38" s="103"/>
+      <c r="C38" s="92"/>
+      <c r="D38" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="57"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="33">
+      <c r="E38" s="52"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="29">
         <v>0.9</v>
       </c>
-      <c r="H38" s="28">
-        <v>1</v>
-      </c>
-      <c r="I38" s="31"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="27">
+        <v>1</v>
+      </c>
+      <c r="I38" s="105"/>
+      <c r="J38" s="30"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="94"/>
-      <c r="C39" s="96"/>
-      <c r="D39" s="30" t="s">
+      <c r="B39" s="103"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="57"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="33">
+      <c r="E39" s="52"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="29">
         <v>0.95</v>
       </c>
-      <c r="H39" s="28">
-        <v>1</v>
-      </c>
-      <c r="I39" s="31"/>
+      <c r="H39" s="27">
+        <v>1</v>
+      </c>
+      <c r="I39" s="105"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="94"/>
-      <c r="C40" s="96"/>
-      <c r="D40" s="30" t="s">
+      <c r="B40" s="103"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="57"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="33">
+      <c r="E40" s="52"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="29">
         <v>0.95</v>
       </c>
-      <c r="H40" s="28">
-        <v>1</v>
-      </c>
-      <c r="I40" s="31"/>
+      <c r="H40" s="27">
+        <v>1</v>
+      </c>
+      <c r="I40" s="105"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="94"/>
-      <c r="C41" s="96"/>
-      <c r="D41" s="30" t="s">
+      <c r="B41" s="103"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="57"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="33">
+      <c r="E41" s="52"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="29">
         <v>0.95</v>
       </c>
-      <c r="H41" s="28">
-        <v>1</v>
-      </c>
-      <c r="I41" s="31"/>
+      <c r="H41" s="27">
+        <v>1</v>
+      </c>
+      <c r="I41" s="105"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="94"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="30" t="s">
+      <c r="B42" s="103"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="57"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="33">
+      <c r="E42" s="52"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="29">
         <v>0.8</v>
       </c>
-      <c r="H42" s="28">
-        <v>1</v>
-      </c>
-      <c r="I42" s="32"/>
+      <c r="H42" s="27">
+        <v>1</v>
+      </c>
+      <c r="I42" s="106"/>
     </row>
     <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="94"/>
-      <c r="C43" s="97"/>
-      <c r="D43" s="36" t="s">
+      <c r="B43" s="103"/>
+      <c r="C43" s="93"/>
+      <c r="D43" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E43" s="59"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="37">
+      <c r="E43" s="54"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="32">
         <v>0.5</v>
       </c>
-      <c r="H43" s="28">
-        <v>1</v>
-      </c>
-      <c r="I43" s="34"/>
+      <c r="H43" s="27">
+        <v>1</v>
+      </c>
+      <c r="I43" s="108"/>
     </row>
     <row r="44" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="38"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="40" t="s">
+      <c r="B44" s="33"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="41"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="36"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="93">
+      <c r="B45" s="110">
         <v>3</v>
       </c>
-      <c r="C45" s="93" t="s">
+      <c r="C45" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="54">
+      <c r="E45" s="49">
         <v>0.9</v>
       </c>
-      <c r="F45" s="54">
+      <c r="F45" s="49">
         <v>0.97</v>
       </c>
-      <c r="G45" s="42">
+      <c r="G45" s="37">
         <v>0.8</v>
       </c>
-      <c r="H45" s="28">
-        <v>1</v>
-      </c>
-      <c r="I45" s="31"/>
+      <c r="H45" s="27">
+        <v>1</v>
+      </c>
+      <c r="I45" s="105"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="99"/>
-      <c r="C46" s="99"/>
-      <c r="D46" s="30" t="s">
+      <c r="B46" s="111"/>
+      <c r="C46" s="94"/>
+      <c r="D46" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="33">
-        <v>1</v>
-      </c>
-      <c r="H46" s="43">
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="29">
+        <v>1</v>
+      </c>
+      <c r="H46" s="38">
         <v>0.98</v>
       </c>
-      <c r="I46" s="31"/>
+      <c r="I46" s="105"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="99"/>
-      <c r="C47" s="99"/>
-      <c r="D47" s="30" t="s">
+      <c r="B47" s="111"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="33">
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="29">
         <v>0.95</v>
       </c>
-      <c r="H47" s="43">
+      <c r="H47" s="38">
         <v>0.98</v>
       </c>
-      <c r="I47" s="31"/>
+      <c r="I47" s="105"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="99"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="30" t="s">
+      <c r="B48" s="111"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="33">
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="29">
         <v>0.5</v>
       </c>
-      <c r="H48" s="43">
+      <c r="H48" s="38">
         <v>0.98</v>
       </c>
-      <c r="I48" s="32"/>
+      <c r="I48" s="106"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="99"/>
-      <c r="C49" s="99"/>
-      <c r="D49" s="30" t="s">
+      <c r="B49" s="111"/>
+      <c r="C49" s="94"/>
+      <c r="D49" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="33">
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="29">
         <v>0.6</v>
       </c>
-      <c r="H49" s="43">
-        <v>1</v>
-      </c>
-      <c r="I49" s="31"/>
+      <c r="H49" s="38">
+        <v>1</v>
+      </c>
+      <c r="I49" s="105"/>
     </row>
     <row r="50" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="100"/>
-      <c r="C50" s="100"/>
-      <c r="D50" s="36" t="s">
+      <c r="B50" s="112"/>
+      <c r="C50" s="95"/>
+      <c r="D50" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="37">
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="32">
         <v>0.8</v>
       </c>
-      <c r="H50" s="44">
+      <c r="H50" s="39">
         <v>0.9</v>
       </c>
-      <c r="I50" s="31"/>
+      <c r="I50" s="105"/>
     </row>
     <row r="51" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="45"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="40" t="s">
+      <c r="B51" s="40"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E51" s="47"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="46"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="48"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="43"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="93">
+      <c r="B52" s="110">
         <v>4</v>
       </c>
-      <c r="C52" s="101" t="s">
+      <c r="C52" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="26" t="s">
+      <c r="D52" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="E52" s="54">
+      <c r="E52" s="49">
         <v>0.98</v>
       </c>
-      <c r="F52" s="54">
+      <c r="F52" s="49">
         <v>0.95</v>
       </c>
-      <c r="G52" s="27">
+      <c r="G52" s="26">
         <v>0.9</v>
       </c>
-      <c r="H52" s="28">
+      <c r="H52" s="27">
         <v>0.98</v>
       </c>
-      <c r="I52" s="31"/>
+      <c r="I52" s="105"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="99"/>
-      <c r="C53" s="96"/>
-      <c r="D53" s="30" t="s">
+      <c r="B53" s="111"/>
+      <c r="C53" s="92"/>
+      <c r="D53" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="33">
-        <v>1</v>
-      </c>
-      <c r="H53" s="43">
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="29">
+        <v>1</v>
+      </c>
+      <c r="H53" s="38">
         <v>0.97</v>
       </c>
-      <c r="I53" s="31"/>
+      <c r="I53" s="105"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="99"/>
-      <c r="C54" s="96"/>
-      <c r="D54" s="30" t="s">
+      <c r="B54" s="111"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="33">
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="29">
         <v>0.9</v>
       </c>
-      <c r="H54" s="43">
+      <c r="H54" s="38">
         <v>0.98</v>
       </c>
-      <c r="I54" s="31"/>
+      <c r="I54" s="105"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="99"/>
-      <c r="C55" s="96"/>
-      <c r="D55" s="30" t="s">
+      <c r="B55" s="111"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="33">
-        <v>1</v>
-      </c>
-      <c r="H55" s="43">
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="29">
+        <v>1</v>
+      </c>
+      <c r="H55" s="38">
         <v>0.97</v>
       </c>
-      <c r="I55" s="31"/>
+      <c r="I55" s="105"/>
     </row>
     <row r="56" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="100"/>
-      <c r="C56" s="97"/>
-      <c r="D56" s="36" t="s">
+      <c r="B56" s="112"/>
+      <c r="C56" s="93"/>
+      <c r="D56" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="37">
+      <c r="E56" s="51"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="32">
         <v>0.9</v>
       </c>
-      <c r="H56" s="44">
-        <v>1</v>
-      </c>
-      <c r="I56" s="31"/>
+      <c r="H56" s="39">
+        <v>1</v>
+      </c>
+      <c r="I56" s="105"/>
     </row>
     <row r="57" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="45"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="40" t="s">
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="46"/>
-      <c r="H57" s="46"/>
-      <c r="I57" s="48"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="41"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="43"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="93">
+      <c r="B58" s="110">
         <v>5</v>
       </c>
-      <c r="C58" s="101" t="s">
+      <c r="C58" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="D58" s="50" t="s">
+      <c r="D58" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="E58" s="54">
+      <c r="E58" s="49">
         <v>0.98</v>
       </c>
-      <c r="F58" s="54">
+      <c r="F58" s="49">
         <v>0.98</v>
       </c>
-      <c r="G58" s="28">
+      <c r="G58" s="27">
         <v>0.95</v>
       </c>
-      <c r="H58" s="28">
+      <c r="H58" s="27">
         <v>0.99</v>
       </c>
-      <c r="I58" s="31"/>
+      <c r="I58" s="105"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="99"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="30" t="s">
+      <c r="B59" s="111"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="33">
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="29">
         <v>0.9</v>
       </c>
-      <c r="H59" s="43">
+      <c r="H59" s="38">
         <v>0.99</v>
       </c>
-      <c r="I59" s="31"/>
+      <c r="I59" s="105"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="99"/>
-      <c r="C60" s="96"/>
-      <c r="D60" s="30" t="s">
+      <c r="B60" s="111"/>
+      <c r="C60" s="92"/>
+      <c r="D60" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="33">
-        <v>1</v>
-      </c>
-      <c r="H60" s="43">
-        <v>1</v>
-      </c>
-      <c r="I60" s="31"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="29">
+        <v>1</v>
+      </c>
+      <c r="H60" s="38">
+        <v>1</v>
+      </c>
+      <c r="I60" s="105"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="99"/>
-      <c r="C61" s="96"/>
-      <c r="D61" s="30" t="s">
+      <c r="B61" s="111"/>
+      <c r="C61" s="92"/>
+      <c r="D61" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="33">
-        <v>1</v>
-      </c>
-      <c r="H61" s="43">
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="29">
+        <v>1</v>
+      </c>
+      <c r="H61" s="38">
         <v>0.98</v>
       </c>
-      <c r="I61" s="31"/>
+      <c r="I61" s="105"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="99"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="30" t="s">
+      <c r="B62" s="111"/>
+      <c r="C62" s="92"/>
+      <c r="D62" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="33">
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="29">
         <v>0.5</v>
       </c>
-      <c r="H62" s="43">
-        <v>1</v>
-      </c>
-      <c r="I62" s="32"/>
+      <c r="H62" s="38">
+        <v>1</v>
+      </c>
+      <c r="I62" s="106"/>
     </row>
     <row r="63" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="100"/>
-      <c r="C63" s="97"/>
-      <c r="D63" s="51" t="s">
+      <c r="B63" s="112"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="44">
+      <c r="E63" s="51"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="39">
         <v>0.5</v>
       </c>
-      <c r="H63" s="44">
-        <v>1</v>
-      </c>
-      <c r="I63" s="32"/>
+      <c r="H63" s="39">
+        <v>1</v>
+      </c>
+      <c r="I63" s="106"/>
     </row>
     <row r="64" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="45"/>
-      <c r="C64" s="46"/>
-      <c r="D64" s="23" t="s">
+      <c r="B64" s="40"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="E64" s="46"/>
-      <c r="F64" s="46"/>
-      <c r="G64" s="46"/>
-      <c r="H64" s="46"/>
-      <c r="I64" s="48"/>
+      <c r="E64" s="41"/>
+      <c r="F64" s="41"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="41"/>
+      <c r="I64" s="43"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" s="93">
+      <c r="B65" s="110">
         <v>6</v>
       </c>
-      <c r="C65" s="101" t="s">
+      <c r="C65" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="D65" s="50" t="s">
+      <c r="D65" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E65" s="54">
+      <c r="E65" s="49">
         <v>0.9</v>
       </c>
-      <c r="F65" s="54">
+      <c r="F65" s="49">
         <v>0.98</v>
       </c>
-      <c r="G65" s="28">
-        <v>1</v>
-      </c>
-      <c r="H65" s="28">
+      <c r="G65" s="27">
+        <v>1</v>
+      </c>
+      <c r="H65" s="27">
         <v>0.99</v>
       </c>
-      <c r="I65" s="31"/>
+      <c r="I65" s="105"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="99"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="30" t="s">
+      <c r="B66" s="111"/>
+      <c r="C66" s="92"/>
+      <c r="D66" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E66" s="55"/>
-      <c r="F66" s="55"/>
-      <c r="G66" s="33">
-        <v>1</v>
-      </c>
-      <c r="H66" s="43">
-        <v>1</v>
-      </c>
-      <c r="I66" s="31"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="29">
+        <v>1</v>
+      </c>
+      <c r="H66" s="38">
+        <v>1</v>
+      </c>
+      <c r="I66" s="105"/>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="99"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="30" t="s">
+      <c r="B67" s="111"/>
+      <c r="C67" s="92"/>
+      <c r="D67" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="33">
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="29">
         <v>0.95</v>
       </c>
-      <c r="H67" s="43">
-        <v>1</v>
-      </c>
-      <c r="I67" s="31"/>
+      <c r="H67" s="38">
+        <v>1</v>
+      </c>
+      <c r="I67" s="105"/>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="99"/>
-      <c r="C68" s="96"/>
-      <c r="D68" s="30" t="s">
+      <c r="B68" s="111"/>
+      <c r="C68" s="92"/>
+      <c r="D68" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="33">
-        <v>1</v>
-      </c>
-      <c r="H68" s="43">
-        <v>1</v>
-      </c>
-      <c r="I68" s="31"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="29">
+        <v>1</v>
+      </c>
+      <c r="H68" s="38">
+        <v>1</v>
+      </c>
+      <c r="I68" s="105"/>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="99"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="30" t="s">
+      <c r="B69" s="111"/>
+      <c r="C69" s="92"/>
+      <c r="D69" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-      <c r="G69" s="33">
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="29">
         <v>0.9</v>
       </c>
-      <c r="H69" s="43">
-        <v>1</v>
-      </c>
-      <c r="I69" s="31"/>
+      <c r="H69" s="38">
+        <v>1</v>
+      </c>
+      <c r="I69" s="105"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="99"/>
-      <c r="C70" s="96"/>
-      <c r="D70" s="30" t="s">
+      <c r="B70" s="111"/>
+      <c r="C70" s="92"/>
+      <c r="D70" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E70" s="55"/>
-      <c r="F70" s="55"/>
-      <c r="G70" s="33">
-        <v>1</v>
-      </c>
-      <c r="H70" s="43">
-        <v>1</v>
-      </c>
-      <c r="I70" s="31"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="29">
+        <v>1</v>
+      </c>
+      <c r="H70" s="38">
+        <v>1</v>
+      </c>
+      <c r="I70" s="105"/>
     </row>
     <row r="71" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="100"/>
-      <c r="C71" s="97"/>
-      <c r="D71" s="51" t="s">
+      <c r="B71" s="112"/>
+      <c r="C71" s="93"/>
+      <c r="D71" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="44">
-        <v>1</v>
-      </c>
-      <c r="H71" s="44">
+      <c r="E71" s="51"/>
+      <c r="F71" s="51"/>
+      <c r="G71" s="39">
+        <v>1</v>
+      </c>
+      <c r="H71" s="39">
         <v>0.99</v>
       </c>
-      <c r="I71" s="31"/>
+      <c r="I71" s="105"/>
     </row>
     <row r="72" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="45"/>
-      <c r="C72" s="46"/>
-      <c r="D72" s="40" t="s">
+      <c r="B72" s="40"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="46"/>
-      <c r="H72" s="46"/>
-      <c r="I72" s="48"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="41"/>
+      <c r="I72" s="43"/>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="93">
+      <c r="B73" s="117">
         <v>7</v>
       </c>
-      <c r="C73" s="101" t="s">
+      <c r="C73" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="D73" s="50" t="s">
+      <c r="D73" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="E73" s="102"/>
-      <c r="F73" s="102"/>
-      <c r="G73" s="28"/>
-      <c r="H73" s="28"/>
-      <c r="I73" s="50"/>
+      <c r="E73" s="49">
+        <v>0.95</v>
+      </c>
+      <c r="F73" s="49">
+        <v>0.95</v>
+      </c>
+      <c r="G73" s="26">
+        <v>1</v>
+      </c>
+      <c r="H73" s="27">
+        <v>0.99</v>
+      </c>
+      <c r="I73" s="105"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="99"/>
-      <c r="C74" s="96"/>
-      <c r="D74" s="30" t="s">
+      <c r="B74" s="118"/>
+      <c r="C74" s="98"/>
+      <c r="D74" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E74" s="102"/>
-      <c r="F74" s="102"/>
-      <c r="G74" s="33"/>
-      <c r="H74" s="43"/>
-      <c r="I74" s="52"/>
+      <c r="E74" s="50"/>
+      <c r="F74" s="50"/>
+      <c r="G74" s="29">
+        <v>1</v>
+      </c>
+      <c r="H74" s="38">
+        <v>0.99</v>
+      </c>
+      <c r="I74" s="105"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="99"/>
-      <c r="C75" s="96"/>
-      <c r="D75" s="52" t="s">
+      <c r="B75" s="118"/>
+      <c r="C75" s="98"/>
+      <c r="D75" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="43"/>
-      <c r="I75" s="52"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="29">
+        <v>1</v>
+      </c>
+      <c r="H75" s="38">
+        <v>0.99</v>
+      </c>
+      <c r="I75" s="105"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="53"/>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="53"/>
+      <c r="B76" s="118"/>
+      <c r="C76" s="98"/>
+      <c r="D76" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="29">
+        <v>1</v>
+      </c>
+      <c r="H76" s="38">
+        <v>0.99</v>
+      </c>
+      <c r="I76" s="105"/>
+    </row>
+    <row r="77" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="119"/>
+      <c r="C77" s="113"/>
+      <c r="D77" s="114" t="s">
+        <v>89</v>
+      </c>
+      <c r="E77" s="51"/>
+      <c r="F77" s="51"/>
+      <c r="G77" s="120">
+        <v>1</v>
+      </c>
+      <c r="H77" s="115">
+        <v>0.99</v>
+      </c>
+      <c r="I77" s="116"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="53"/>
+      <c r="B78" s="48"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="53"/>
+      <c r="B79" s="48"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="53"/>
+      <c r="B80" s="48"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="53"/>
+      <c r="B81" s="48"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="53"/>
+      <c r="B82" s="48"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="53"/>
+      <c r="B83" s="48"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="53"/>
+      <c r="B84" s="48"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="53"/>
+      <c r="B85" s="48"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="53"/>
+      <c r="B86" s="48"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="53"/>
+      <c r="B87" s="48"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="53"/>
+      <c r="B88" s="48"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="53"/>
+      <c r="B89" s="48"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="53"/>
+      <c r="B90" s="48"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="53"/>
+      <c r="B91" s="48"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="53"/>
+      <c r="B92" s="48"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="53"/>
+      <c r="B93" s="48"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="53"/>
+      <c r="B94" s="48"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="53"/>
+      <c r="B95" s="48"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="53"/>
+      <c r="B96" s="48"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="53"/>
+      <c r="B97" s="48"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="53"/>
+      <c r="B98" s="48"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="53"/>
+      <c r="B99" s="48"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="53"/>
+      <c r="B100" s="48"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="53"/>
+      <c r="B101" s="48"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="53"/>
+      <c r="B102" s="48"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="53"/>
+      <c r="B103" s="48"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="53"/>
+      <c r="B104" s="48"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="53"/>
+      <c r="B105" s="48"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="53"/>
+      <c r="B106" s="48"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="53"/>
+      <c r="B107" s="48"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="53"/>
+      <c r="B108" s="48"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="53"/>
+      <c r="B109" s="48"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="53"/>
+      <c r="B110" s="48"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="53"/>
+      <c r="B111" s="48"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="53"/>
+      <c r="B112" s="48"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="53"/>
+      <c r="B113" s="48"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="53"/>
+      <c r="B114" s="48"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="53"/>
+      <c r="B115" s="48"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="53"/>
+      <c r="B116" s="48"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="53"/>
+      <c r="B117" s="48"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="53"/>
+      <c r="B118" s="48"/>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="53"/>
+      <c r="B119" s="48"/>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="53"/>
+      <c r="B120" s="48"/>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="53"/>
+      <c r="B121" s="48"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="53"/>
+      <c r="B122" s="48"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="53"/>
+      <c r="B123" s="48"/>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="53"/>
+      <c r="B124" s="48"/>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="53"/>
+      <c r="B125" s="48"/>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="53"/>
+      <c r="B126" s="48"/>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="53"/>
+      <c r="B127" s="48"/>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="53"/>
+      <c r="B128" s="48"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="53"/>
+      <c r="B129" s="48"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="53"/>
+      <c r="B130" s="48"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="53"/>
+      <c r="B131" s="48"/>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="53"/>
+      <c r="B132" s="48"/>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="53"/>
+      <c r="B133" s="48"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="53"/>
+      <c r="B134" s="48"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="53"/>
+      <c r="B135" s="48"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="53"/>
+      <c r="B136" s="48"/>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="53"/>
+      <c r="B137" s="48"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="53"/>
+      <c r="B138" s="48"/>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="53"/>
+      <c r="B139" s="48"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="53"/>
+      <c r="B140" s="48"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="53"/>
+      <c r="B141" s="48"/>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="53"/>
+      <c r="B142" s="48"/>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="53"/>
+      <c r="B143" s="48"/>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="53"/>
+      <c r="B144" s="48"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="53"/>
+      <c r="B145" s="48"/>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="53"/>
+      <c r="B146" s="48"/>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="53"/>
+      <c r="B147" s="48"/>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="53"/>
+      <c r="B148" s="48"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="53"/>
+      <c r="B149" s="48"/>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="53"/>
+      <c r="B150" s="48"/>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="53"/>
+      <c r="B151" s="48"/>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="53"/>
+      <c r="B152" s="48"/>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="53"/>
+      <c r="B153" s="48"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="53"/>
+      <c r="B154" s="48"/>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="53"/>
+      <c r="B155" s="48"/>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="53"/>
+      <c r="B156" s="48"/>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="53"/>
+      <c r="B157" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="C73:C75"/>
+  <mergeCells count="39">
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="B73:B77"/>
+    <mergeCell ref="E73:E77"/>
+    <mergeCell ref="F73:F77"/>
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="C52:C56"/>
     <mergeCell ref="B58:B63"/>
@@ -3117,6 +3450,7 @@
     <mergeCell ref="E65:E71"/>
     <mergeCell ref="F65:F71"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>